<commit_message>
fix tagihan spp, tagihan biasa dan lainnya
</commit_message>
<xml_diff>
--- a/import/TK-B1-2-1-2019.xlsx.xlsx
+++ b/import/TK-B1-2-1-2019.xlsx.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
   <si>
     <t>Kode Siswa</t>
   </si>
@@ -73,18 +73,6 @@
   </si>
   <si>
     <t>Azka Syadaad Emiraldi Novriansyah</t>
-  </si>
-  <si>
-    <t>2-1-141021</t>
-  </si>
-  <si>
-    <t>Badranaya Aksa Wijaya</t>
-  </si>
-  <si>
-    <t>2-1-141042</t>
-  </si>
-  <si>
-    <t>Made Ngurah Prabha Laksmana</t>
   </si>
   <si>
     <t>2-1-141050</t>
@@ -479,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +518,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -553,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -576,7 +564,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -599,7 +587,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -616,13 +604,13 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>141021</v>
+        <v>141050</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -636,16 +624,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>141042</v>
+        <v>141050</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -659,16 +647,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>141050</v>
+        <v>141031</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -685,13 +673,13 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>141050</v>
+        <v>141045</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -708,13 +696,13 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>141031</v>
+        <v>141037</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -731,13 +719,13 @@
         <v>26</v>
       </c>
       <c r="B11">
-        <v>141045</v>
+        <v>141039</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -751,16 +739,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>141037</v>
+        <v>141039</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -774,16 +762,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13">
-        <v>141039</v>
+        <v>141041</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -800,13 +788,13 @@
         <v>30</v>
       </c>
       <c r="B14">
-        <v>141039</v>
+        <v>141043</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -823,13 +811,13 @@
         <v>32</v>
       </c>
       <c r="B15">
-        <v>141041</v>
+        <v>141034</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -843,17 +831,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>141043</v>
+        <v>141053</v>
       </c>
       <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
@@ -861,52 +849,6 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17">
-        <v>141034</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>141053</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>